<commit_message>
addred roles using normalization
</commit_message>
<xml_diff>
--- a/assets/excel/address_list.xlsx
+++ b/assets/excel/address_list.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
   <si>
     <t/>
   </si>
@@ -50,85 +50,82 @@
     <t>Image</t>
   </si>
   <si>
-    <t>Hobbies</t>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Mrs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xyz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Popz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Karunagappally</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> samp@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> default_user30.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Manager</t>
+  </si>
+  <si>
+    <t>Driver</t>
   </si>
   <si>
     <t>Mr.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Sample</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Contact</t>
+    <t xml:space="preserve"> Edited2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> S</t>
   </si>
   <si>
     <t xml:space="preserve"> Male</t>
   </si>
   <si>
-    <t xml:space="preserve">  Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sample@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sample23.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sports</t>
-  </si>
-  <si>
-    <t>painting</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> test@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Anujith.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> reading</t>
-  </si>
-  <si>
-    <t>writting</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> New Edited</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> example@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> default_user.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> videogames</t>
-  </si>
-  <si>
-    <t>Mrs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TestStreet</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> chumma@gmail.com</t>
-  </si>
-  <si>
-    <t>reading</t>
-  </si>
-  <si>
-    <t>learning</t>
+    <t xml:space="preserve"> Mynagappally</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vazhappallilthekkathil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> edited1@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sample.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Driver</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AnujithEdited</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> anujithtest13@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ABC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> testdata@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -180,27 +177,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="5.09765625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.83984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.43359375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="8.05078125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.4609375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="10.73828125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="8.69921875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="20.5703125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="15.32421875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="21.2421875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="24.70703125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="14.5859375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="8.171875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="16.78125" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="12.2421875" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="8.33984375" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="8.05078125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="8.30859375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="19.01171875" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="9.57421875" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="6.8828125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -255,7 +250,7 @@
         <v>16</v>
       </c>
       <c r="E2" t="n" s="1">
-        <v>45506.0</v>
+        <v>45573.0</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -284,101 +279,98 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E3" t="n" s="1">
-        <v>45539.0</v>
+        <v>45568.0</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I3" t="n">
-        <v>1.111111111E9</v>
+        <v>9.048503717E9</v>
       </c>
       <c r="J3" t="n">
-        <v>999999.0</v>
+        <v>690500.0</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="n" s="1">
+        <v>45567.0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="n" s="1">
-        <v>45513.0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I4" t="n">
-        <v>1.111111111E9</v>
+        <v>9.048503717E9</v>
       </c>
       <c r="J4" t="n">
-        <v>999999.0</v>
+        <v>690500.0</v>
       </c>
       <c r="K4" t="s">
         <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E5" t="n" s="1">
-        <v>45506.0</v>
+        <v>45573.0</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
@@ -387,25 +379,19 @@
         <v>36</v>
       </c>
       <c r="I5" t="n">
-        <v>2.222222222E9</v>
+        <v>9.875987543E9</v>
       </c>
       <c r="J5" t="n">
-        <v>222222.0</v>
+        <v>999999.0</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L5" t="s">
         <v>31</v>
       </c>
       <c r="M5" t="s">
         <v>37</v>
-      </c>
-      <c r="N5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>